<commit_message>
renaming and file structure setting up forms
</commit_message>
<xml_diff>
--- a/tablesetup.xlsx
+++ b/tablesetup.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Assignments</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>article</t>
+  </si>
+  <si>
+    <t>Samwise</t>
+  </si>
+  <si>
+    <t>Ohio Nick</t>
   </si>
 </sst>
 </file>
@@ -290,7 +296,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -306,8 +312,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -327,8 +335,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -336,6 +351,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -343,6 +359,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -672,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:P28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -683,31 +700,33 @@
     <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.1640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="2.33203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="2"/>
-    <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="2.6640625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="2.1640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.33203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="2"/>
+    <col min="14" max="14" width="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.6640625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="46" customHeight="1">
+    <row r="1" spans="1:9" ht="46" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="4" t="s">
+      <c r="D1" s="11"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="G1" s="4"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -717,17 +736,18 @@
       <c r="C2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2"/>
       <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -737,61 +757,65 @@
       <c r="C3" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3">
+      <c r="D3" s="12"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="3">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="3">
+      <c r="E4" s="2"/>
+      <c r="F4" s="3">
         <v>2</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="3">
+      <c r="E5" s="2"/>
+      <c r="F5" s="3">
         <v>3</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="2"/>
       <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
       <c r="B6" s="7"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="3">
+      <c r="E6" s="2"/>
+      <c r="F6" s="3">
         <v>4</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -800,16 +824,17 @@
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="3">
+      <c r="E7" s="2"/>
+      <c r="F7" s="3">
         <v>5</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="3">
         <v>1</v>
       </c>
@@ -818,16 +843,17 @@
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="3">
+      <c r="E8" s="2"/>
+      <c r="F8" s="3">
         <v>6</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="3">
         <v>2</v>
       </c>
@@ -836,43 +862,45 @@
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="3">
+      <c r="E9" s="2"/>
+      <c r="F9" s="3">
         <v>7</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="D10" s="2"/>
-      <c r="E10" s="3">
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="E10" s="2"/>
+      <c r="F10" s="3">
         <v>8</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="3">
+      <c r="D11" s="8"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="3">
         <v>9</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -882,17 +910,20 @@
       <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="3">
+      <c r="D12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="3">
         <v>10</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="3">
         <v>1</v>
       </c>
@@ -902,61 +933,67 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="3">
+      <c r="D13" s="3">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="3">
         <v>11</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="3">
+      <c r="E14" s="2"/>
+      <c r="F14" s="3">
         <v>12</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="3">
+      <c r="E15" s="2"/>
+      <c r="F15" s="3">
         <v>13</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="2"/>
       <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="3">
+      <c r="E16" s="2"/>
+      <c r="F16" s="3">
         <v>14</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
@@ -965,16 +1002,17 @@
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
-      <c r="E17" s="3">
+      <c r="E17" s="2"/>
+      <c r="F17" s="3">
         <v>15</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" s="3">
         <v>5</v>
       </c>
@@ -983,16 +1021,17 @@
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="3">
+      <c r="E18" s="2"/>
+      <c r="F18" s="3">
         <v>16</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" s="3">
         <v>6</v>
       </c>
@@ -1001,16 +1040,17 @@
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-      <c r="E19" s="3">
+      <c r="E19" s="2"/>
+      <c r="F19" s="3">
         <v>17</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" s="3">
         <v>7</v>
       </c>
@@ -1019,30 +1059,32 @@
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="3">
+      <c r="E20" s="2"/>
+      <c r="F20" s="3">
         <v>18</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20" s="2"/>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="3">
+      <c r="E21" s="2"/>
+      <c r="F21" s="3">
         <v>19</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21" s="2"/>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1051,8 +1093,9 @@
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1061,8 +1104,9 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23" s="2"/>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1071,8 +1115,9 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24" s="2"/>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1081,8 +1126,9 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25" s="2"/>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1091,8 +1137,9 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26" s="2"/>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1101,8 +1148,9 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27" s="2"/>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1111,13 +1159,14 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A11:D11"/>
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>